<commit_message>
adding new fqs names
</commit_message>
<xml_diff>
--- a/dataset_desc.xlsx
+++ b/dataset_desc.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,1542 +360,1682 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Accession</t>
+          <t>SRX</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>SRX</t>
+          <t>SRR</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>SRR</t>
+          <t>omic</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>omic</t>
+          <t>condition</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>condition</t>
+          <t>replicate</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>replicate</t>
+          <t>sample</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>sample</t>
+          <t>lane</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>lane</t>
+          <t>description</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>rep</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>rep</t>
+          <t>cond</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>cond</t>
+          <t>F4</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>R1</t>
+          <t>F3</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>R2</t>
+          <t>F2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>F1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>GSM6543819</t>
+          <t>SRX17944178</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SRX17944178</t>
+          <t>SRR21960687</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SRR21960687</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>rep1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>REP1_HLTY</t>
-        </is>
-      </c>
-      <c r="H2">
+          <t>S1HLTY</t>
+        </is>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 1</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>REP1</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR21960687_4.fastq.gz -&gt; SRR21960687_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>./SRR21960687_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR21960687_3.fastq.gz -&gt; SRR21960687_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>./SRR21960687_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR21960687_2.fastq.gz -&gt; SRR21960687_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>SRR21960687_1.fastq.gz -&gt; SRR21960687_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GSM6543819</t>
+          <t>SRX17944178</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SRX17944178</t>
+          <t>SRR21960688</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SRR21960688</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>rep1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>REP1_HLTY</t>
-        </is>
-      </c>
-      <c r="H3">
+          <t>S1HLTY</t>
+        </is>
+      </c>
+      <c r="G3">
         <v>2</v>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 1</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>REP1</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR21960688_4.fastq.gz -&gt; SRR21960688_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>./SRR21960688_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR21960688_3.fastq.gz -&gt; SRR21960688_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>./SRR21960688_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR21960688_2.fastq.gz -&gt; SRR21960688_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>SRR21960688_1.fastq.gz -&gt; SRR21960688_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GSM6543820</t>
+          <t>SRX17944179</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SRX17944179</t>
+          <t>SRR21960685</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SRR21960685</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep2</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>rep2</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>REP2_HLTY</t>
-        </is>
-      </c>
-      <c r="H4">
+          <t>S2HLTY</t>
+        </is>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 2</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>REP2</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR21960685_4.fastq.gz -&gt; SRR21960685_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>./SRR21960685_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR21960685_3.fastq.gz -&gt; SRR21960685_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>./SRR21960685_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR21960685_2.fastq.gz -&gt; SRR21960685_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>SRR21960685_1.fastq.gz -&gt; SRR21960685_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GSM6543820</t>
+          <t>SRX17944179</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SRX17944179</t>
+          <t>SRR21960686</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SRR21960686</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>rep2</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>REP2_HLTY</t>
-        </is>
-      </c>
-      <c r="H5">
+          <t>S2HLTY</t>
+        </is>
+      </c>
+      <c r="G5">
         <v>2</v>
       </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 2</t>
+        </is>
+      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>REP2</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR21960686_4.fastq.gz -&gt; SRR21960686_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>./SRR21960686_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR21960686_3.fastq.gz -&gt; SRR21960686_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>./SRR21960686_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR21960686_2.fastq.gz -&gt; SRR21960686_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>SRR21960686_1.fastq.gz -&gt; SRR21960686_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GSM6543821</t>
+          <t>SRX17944180</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SRX17944180</t>
+          <t>SRR21960683</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SRR21960683</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>rep3</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>REP3_HLTY</t>
-        </is>
-      </c>
-      <c r="H6">
+          <t>S3HLTY</t>
+        </is>
+      </c>
+      <c r="G6">
         <v>1</v>
       </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 3</t>
+        </is>
+      </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 3</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>REP3</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR21960683_4.fastq.gz -&gt; SRR21960683_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>./SRR21960683_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR21960683_3.fastq.gz -&gt; SRR21960683_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>./SRR21960683_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR21960683_2.fastq.gz -&gt; SRR21960683_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>SRR21960683_1.fastq.gz -&gt; SRR21960683_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GSM6543821</t>
+          <t>SRX17944180</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SRX17944180</t>
+          <t>SRR21960684</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SRR21960684</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep3</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>rep3</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>REP3_HLTY</t>
-        </is>
-      </c>
-      <c r="H7">
+          <t>S3HLTY</t>
+        </is>
+      </c>
+      <c r="G7">
         <v>2</v>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 3</t>
+        </is>
+      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome (scRNA-seq + scATAC-seq) biological replicate 3</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>REP3</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR21960684_4.fastq.gz -&gt; SRR21960684_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>./SRR21960684_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR21960684_3.fastq.gz -&gt; SRR21960684_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>./SRR21960684_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR21960684_2.fastq.gz -&gt; SRR21960684_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>SRR21960684_1.fastq.gz -&gt; SRR21960684_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>GSM6543822</t>
+          <t>SRX17944181</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SRX17944181</t>
+          <t>SRR21960681</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SRR21960681</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep1</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>rep1</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>REP1_CNCR</t>
-        </is>
-      </c>
-      <c r="H8">
+          <t>S1CNCR</t>
+        </is>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 1</t>
+        </is>
+      </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>REP1</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR21960681_4.fastq.gz -&gt; SRR21960681_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>./SRR21960681_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR21960681_3.fastq.gz -&gt; SRR21960681_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>./SRR21960681_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR21960681_2.fastq.gz -&gt; SRR21960681_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>SRR21960681_1.fastq.gz -&gt; SRR21960681_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GSM6543822</t>
+          <t>SRX17944181</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SRX17944181</t>
+          <t>SRR21960682</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>SRR21960682</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep1</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>rep1</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>REP1_CNCR</t>
-        </is>
-      </c>
-      <c r="H9">
+          <t>S1CNCR</t>
+        </is>
+      </c>
+      <c r="G9">
         <v>2</v>
       </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 1</t>
+        </is>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>REP1</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR21960682_4.fastq.gz -&gt; SRR21960682_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>./SRR21960682_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR21960682_3.fastq.gz -&gt; SRR21960682_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>./SRR21960682_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR21960682_2.fastq.gz -&gt; SRR21960682_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>SRR21960682_1.fastq.gz -&gt; SRR21960682_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GSM6543823</t>
+          <t>SRX17944182</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SRX17944182</t>
+          <t>SRR21960679</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>SRR21960679</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep2</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>rep2</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>REP2_CNCR</t>
-        </is>
-      </c>
-      <c r="H10">
+          <t>S2CNCR</t>
+        </is>
+      </c>
+      <c r="G10">
         <v>1</v>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 2</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>REP2</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR21960679_4.fastq.gz -&gt; SRR21960679_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>./SRR21960679_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR21960679_3.fastq.gz -&gt; SRR21960679_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>./SRR21960679_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR21960679_2.fastq.gz -&gt; SRR21960679_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>SRR21960679_1.fastq.gz -&gt; SRR21960679_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>GSM6543823</t>
+          <t>SRX17944182</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SRX17944182</t>
+          <t>SRR21960680</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>SRR21960680</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep2</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>rep2</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>REP2_CNCR</t>
-        </is>
-      </c>
-      <c r="H11">
+          <t>S2CNCR</t>
+        </is>
+      </c>
+      <c r="G11">
         <v>2</v>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 2</t>
+        </is>
+      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>REP2</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR21960680_4.fastq.gz -&gt; SRR21960680_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>./SRR21960680_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR21960680_3.fastq.gz -&gt; SRR21960680_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>./SRR21960680_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR21960680_2.fastq.gz -&gt; SRR21960680_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>SRR21960680_1.fastq.gz -&gt; SRR21960680_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>GSM6543824</t>
+          <t>SRX17944183</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SRX17944183</t>
+          <t>SRR21960678</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>SRR21960678</t>
+          <t>scRNAseq</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>scRNAseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep3</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>rep3</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>REP3_CNCR</t>
-        </is>
-      </c>
-      <c r="H12">
+          <t>S3CNCR</t>
+        </is>
+      </c>
+      <c r="G12">
         <v>1</v>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 3</t>
+        </is>
+      </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome (scRNA-seq + scATAC-seq) early stage biological replicate 3</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>REP3</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR21960678_4.fastq.gz -&gt; SRR21960678_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>./SRR21960678_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR21960678_3.fastq.gz -&gt; SRR21960678_S1_L001_I2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>./SRR21960678_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR21960678_2.fastq.gz -&gt; SRR21960678_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>SRR21960678_1.fastq.gz -&gt; SRR21960678_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GSM6774763</t>
+          <t>SRX18447852</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SRX18447852</t>
+          <t>SRR22482677</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>SRR22482677</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep1</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>rep1</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>REP1_HLTY</t>
-        </is>
-      </c>
-      <c r="H13">
+          <t>S1HLTY</t>
+        </is>
+      </c>
+      <c r="G13">
         <v>1</v>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 1</t>
+        </is>
+      </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>REP1</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR22482677_4.fastq.gz -&gt; SRR22482677_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>./SRR22482677_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR22482677_3.fastq.gz -&gt; SRR22482677_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>./SRR22482677_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR22482677_2.fastq.gz -&gt; SRR22482677_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>SRR22482677_1.fastq.gz -&gt; SRR22482677_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GSM6774763</t>
+          <t>SRX18447852</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SRX18447852</t>
+          <t>SRR22482678</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>SRR22482678</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep1</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>rep1</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>REP1_HLTY</t>
-        </is>
-      </c>
-      <c r="H14">
+          <t>S1HLTY</t>
+        </is>
+      </c>
+      <c r="G14">
         <v>2</v>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 1</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>REP1</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR22482678_4.fastq.gz -&gt; SRR22482678_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>./SRR22482678_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR22482678_3.fastq.gz -&gt; SRR22482678_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>./SRR22482678_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR22482678_2.fastq.gz -&gt; SRR22482678_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>SRR22482678_1.fastq.gz -&gt; SRR22482678_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GSM6774764</t>
+          <t>SRX18447853</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SRX18447853</t>
+          <t>SRR22482675</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SRR22482675</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep2</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>rep2</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>REP2_HLTY</t>
-        </is>
-      </c>
-      <c r="H15">
+          <t>S2HLTY</t>
+        </is>
+      </c>
+      <c r="G15">
         <v>1</v>
       </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 2</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>REP2</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR22482675_4.fastq.gz -&gt; SRR22482675_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>./SRR22482675_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR22482675_3.fastq.gz -&gt; SRR22482675_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>./SRR22482675_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR22482675_2.fastq.gz -&gt; SRR22482675_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>SRR22482675_1.fastq.gz -&gt; SRR22482675_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GSM6774764</t>
+          <t>SRX18447853</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SRX18447853</t>
+          <t>SRR22482676</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>SRR22482676</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep2</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>rep2</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>REP2_HLTY</t>
-        </is>
-      </c>
-      <c r="H16">
+          <t>S2HLTY</t>
+        </is>
+      </c>
+      <c r="G16">
         <v>2</v>
       </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 2</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>REP2</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR22482676_4.fastq.gz -&gt; SRR22482676_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>./SRR22482676_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR22482676_3.fastq.gz -&gt; SRR22482676_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>./SRR22482676_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR22482676_2.fastq.gz -&gt; SRR22482676_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>SRR22482676_1.fastq.gz -&gt; SRR22482676_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GSM6774765</t>
+          <t>SRX18447854</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SRX18447854</t>
+          <t>SRR22482673</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SRR22482673</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep3</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>rep3</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>REP3_HLTY</t>
-        </is>
-      </c>
-      <c r="H17">
+          <t>S3HLTY</t>
+        </is>
+      </c>
+      <c r="G17">
         <v>1</v>
       </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 3</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 3</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>REP3</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR22482673_4.fastq.gz -&gt; SRR22482673_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>./SRR22482673_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR22482673_3.fastq.gz -&gt; SRR22482673_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>./SRR22482673_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR22482673_2.fastq.gz -&gt; SRR22482673_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>SRR22482673_1.fastq.gz -&gt; SRR22482673_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GSM6774765</t>
+          <t>SRX18447854</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SRX18447854</t>
+          <t>SRR22482674</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>SRR22482674</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>healthy</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>healthy</t>
+          <t>rep3</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>rep3</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>REP3_HLTY</t>
-        </is>
-      </c>
-      <c r="H18">
+          <t>S3HLTY</t>
+        </is>
+      </c>
+      <c r="G18">
         <v>2</v>
       </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 3</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>mouse breast (non-cancer) multiome scATAC-seq raw data biological replicate 3</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>REP3</t>
+          <t>HLTY</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>HLTY</t>
+          <t>SRR22482674_4.fastq.gz -&gt; SRR22482674_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>./SRR22482674_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR22482674_3.fastq.gz -&gt; SRR22482674_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>./SRR22482674_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR22482674_2.fastq.gz -&gt; SRR22482674_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>SRR22482674_1.fastq.gz -&gt; SRR22482674_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>GSM6774766</t>
+          <t>SRX18447855</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SRX18447855</t>
+          <t>SRR22482671</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SRR22482671</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep1</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>rep1</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>REP1_CNCR</t>
-        </is>
-      </c>
-      <c r="H19">
+          <t>S1CNCR</t>
+        </is>
+      </c>
+      <c r="G19">
         <v>1</v>
       </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 1</t>
+        </is>
+      </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>REP1</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR22482671_4.fastq.gz -&gt; SRR22482671_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>./SRR22482671_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR22482671_3.fastq.gz -&gt; SRR22482671_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>./SRR22482671_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR22482671_2.fastq.gz -&gt; SRR22482671_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>SRR22482671_1.fastq.gz -&gt; SRR22482671_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GSM6774766</t>
+          <t>SRX18447855</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SRX18447855</t>
+          <t>SRR22482672</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SRR22482672</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep1</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>rep1</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>REP1_CNCR</t>
-        </is>
-      </c>
-      <c r="H20">
+          <t>S1CNCR</t>
+        </is>
+      </c>
+      <c r="G20">
         <v>2</v>
       </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 1</t>
+        </is>
+      </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 1</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>REP1</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR22482672_4.fastq.gz -&gt; SRR22482672_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>./SRR22482672_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR22482672_3.fastq.gz -&gt; SRR22482672_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>./SRR22482672_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR22482672_2.fastq.gz -&gt; SRR22482672_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>SRR22482672_1.fastq.gz -&gt; SRR22482672_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GSM6774767</t>
+          <t>SRX18447856</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SRX18447856</t>
+          <t>SRR22482668</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SRR22482668</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep2</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>rep2</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>REP2_CNCR</t>
-        </is>
-      </c>
-      <c r="H21">
+          <t>S2CNCR</t>
+        </is>
+      </c>
+      <c r="G21">
         <v>1</v>
       </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 2</t>
+        </is>
+      </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>REP2</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR22482668_4.fastq.gz -&gt; SRR22482668_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>./SRR22482668_S1_L001_R1_001.fastq.gz</t>
+          <t>SRR22482668_3.fastq.gz -&gt; SRR22482668_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>./SRR22482668_S1_L001_R2_001.fastq.gz</t>
+          <t>SRR22482668_2.fastq.gz -&gt; SRR22482668_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>SRR22482668_1.fastq.gz -&gt; SRR22482668_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GSM6774767</t>
+          <t>SRX18447856</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SRX18447856</t>
+          <t>SRR22482669</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>SRR22482669</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>rep2</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>REP2_CNCR</t>
-        </is>
-      </c>
-      <c r="H22">
+          <t>S2CNCR</t>
+        </is>
+      </c>
+      <c r="G22">
         <v>2</v>
       </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 2</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 2</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>REP2</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR22482669_4.fastq.gz -&gt; SRR22482669_S1_L001_R3_001.fastq.gz</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>./SRR22482669_S1_L002_R1_001.fastq.gz</t>
+          <t>SRR22482669_3.fastq.gz -&gt; SRR22482669_S1_L001_R2_001.fastq.gz</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>./SRR22482669_S1_L002_R2_001.fastq.gz</t>
+          <t>SRR22482669_2.fastq.gz -&gt; SRR22482669_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>SRR22482669_1.fastq.gz -&gt; SRR22482669_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GSM6774768</t>
+          <t>SRX18447857</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SRX18447857</t>
+          <t>SRR22482666</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SRR22482666</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep3</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>rep3</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>REP3_CNCR</t>
-        </is>
-      </c>
-      <c r="H23">
+          <t>S3CNCR</t>
+        </is>
+      </c>
+      <c r="G23">
         <v>1</v>
       </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 3</t>
+        </is>
+      </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 3</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>REP3</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR22482666_4.fastq.gz -&gt; SRR22482666_S1_L001_R3_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>SRR22482666_3.fastq.gz -&gt; SRR22482666_S1_L001_R2_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>SRR22482666_2.fastq.gz -&gt; SRR22482666_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>SRR22482666_1.fastq.gz -&gt; SRR22482666_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GSM6774768</t>
+          <t>SRX18447857</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SRX18447857</t>
+          <t>SRR22482667</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SRR22482667</t>
+          <t>scATACseq</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>scATACseq</t>
+          <t>cancer</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>cancer</t>
+          <t>rep3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>rep3</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>REP3_CNCR</t>
-        </is>
-      </c>
-      <c r="H24">
+          <t>S3CNCR</t>
+        </is>
+      </c>
+      <c r="G24">
         <v>2</v>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 3</t>
+        </is>
+      </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>mouse breast cancer multiome scATAC-seq raw data early stage biological replicate 3</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>REP3</t>
+          <t>CNCR</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>CNCR</t>
+          <t>SRR22482667_4.fastq.gz -&gt; SRR22482667_S1_L001_R3_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>SRR22482667_3.fastq.gz -&gt; SRR22482667_S1_L001_R2_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>SRR22482667_2.fastq.gz -&gt; SRR22482667_S1_L001_R1_001.fastq.gz</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>SRR22482667_1.fastq.gz -&gt; SRR22482667_S1_L001_I1_001.fastq.gz</t>
         </is>
       </c>
     </row>

</xml_diff>